<commit_message>
Image save 기능 구현
</commit_message>
<xml_diff>
--- a/NotchingGradeInsp_Document/SPC+/LHM_EXCEL_작업/SPCPlus_클래스정의.xlsx
+++ b/NotchingGradeInsp_Document/SPC+/LHM_EXCEL_작업/SPCPlus_클래스정의.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="28035" windowHeight="12570" tabRatio="779" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="28035" windowHeight="12570" tabRatio="779" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="클래스정보" sheetId="9" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Alarm Class 생성 정보" sheetId="5" r:id="rId5"/>
     <sheet name="Spec_Para Class 생성 정보" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="573">
   <si>
     <t>클래스명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -309,14 +309,6 @@
   </si>
   <si>
     <t>m_DefectCameraLocation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>m_DefectCameraNumber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>m_DefectScreenNumber</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2255,6 +2247,30 @@
   </si>
   <si>
     <t>//Image 기준 불량 발생 위치 Y [pxl]_절대 위치 Image좌,상단(0,0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_DefectScreenNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_DefectCameraNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_CameraLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_CameraNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m_ScreenNumber</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2973,7 +2989,7 @@
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="38" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -2994,7 +3010,7 @@
       <c r="R1" s="39"/>
       <c r="S1" s="40"/>
       <c r="T1" s="38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U1" s="39"/>
       <c r="V1" s="39"/>
@@ -3024,7 +3040,7 @@
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="23" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -3036,7 +3052,7 @@
       <c r="K2" s="25"/>
       <c r="L2" s="14"/>
       <c r="M2" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
@@ -3046,7 +3062,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
@@ -3083,7 +3099,7 @@
       <c r="K3" s="28"/>
       <c r="L3" s="17"/>
       <c r="M3" s="18" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
@@ -3093,7 +3109,7 @@
       <c r="S3" s="19"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="V3" s="18"/>
       <c r="W3" s="18"/>
@@ -3130,7 +3146,7 @@
       <c r="K4" s="28"/>
       <c r="L4" s="17"/>
       <c r="M4" s="18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
@@ -3140,7 +3156,7 @@
       <c r="S4" s="19"/>
       <c r="T4" s="18"/>
       <c r="U4" s="18" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="V4" s="18"/>
       <c r="W4" s="18"/>
@@ -3177,7 +3193,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="17"/>
       <c r="M5" s="18" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
@@ -3187,7 +3203,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="18"/>
       <c r="U5" s="18" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
@@ -3224,7 +3240,7 @@
       <c r="K6" s="31"/>
       <c r="L6" s="20"/>
       <c r="M6" s="21" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
@@ -3234,7 +3250,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="21"/>
       <c r="U6" s="21" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="V6" s="21"/>
       <c r="W6" s="21"/>
@@ -3263,7 +3279,7 @@
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="23" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
@@ -3275,7 +3291,7 @@
       <c r="K7" s="25"/>
       <c r="L7" s="14"/>
       <c r="M7" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -3285,7 +3301,7 @@
       <c r="S7" s="16"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
@@ -3322,7 +3338,7 @@
       <c r="K8" s="31"/>
       <c r="L8" s="20"/>
       <c r="M8" s="21" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
@@ -3332,7 +3348,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
@@ -3361,7 +3377,7 @@
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="23" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -3373,7 +3389,7 @@
       <c r="K9" s="25"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -3383,7 +3399,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
@@ -3420,7 +3436,7 @@
       <c r="K10" s="28"/>
       <c r="L10" s="5"/>
       <c r="M10" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -3430,7 +3446,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
@@ -3467,7 +3483,7 @@
       <c r="K11" s="31"/>
       <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -3477,7 +3493,7 @@
       <c r="S11" s="10"/>
       <c r="T11" s="9"/>
       <c r="U11" s="9" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -3506,7 +3522,7 @@
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="41" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
@@ -3518,7 +3534,7 @@
       <c r="K12" s="43"/>
       <c r="L12" s="13"/>
       <c r="M12" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
@@ -3528,7 +3544,7 @@
       <c r="S12" s="12"/>
       <c r="T12" s="11"/>
       <c r="U12" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
@@ -3557,7 +3573,7 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
@@ -3569,7 +3585,7 @@
       <c r="K13" s="43"/>
       <c r="L13" s="13"/>
       <c r="M13" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
@@ -3579,7 +3595,7 @@
       <c r="S13" s="12"/>
       <c r="T13" s="11"/>
       <c r="U13" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
@@ -3608,7 +3624,7 @@
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="23" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
@@ -3620,7 +3636,7 @@
       <c r="K14" s="25"/>
       <c r="L14" s="14"/>
       <c r="M14" s="15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
@@ -3630,7 +3646,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="15"/>
       <c r="U14" s="15" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="V14" s="15"/>
       <c r="W14" s="15"/>
@@ -3667,7 +3683,7 @@
       <c r="K15" s="28"/>
       <c r="L15" s="17"/>
       <c r="M15" s="18" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
@@ -3677,7 +3693,7 @@
       <c r="S15" s="19"/>
       <c r="T15" s="18"/>
       <c r="U15" s="18" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
@@ -3714,7 +3730,7 @@
       <c r="K16" s="31"/>
       <c r="L16" s="20"/>
       <c r="M16" s="21" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
@@ -3724,7 +3740,7 @@
       <c r="S16" s="22"/>
       <c r="T16" s="21"/>
       <c r="U16" s="21" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="V16" s="21"/>
       <c r="W16" s="21"/>
@@ -3805,7 +3821,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3813,16 +3829,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2" t="s">
         <v>405</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>407</v>
       </c>
-      <c r="D2" t="s">
-        <v>409</v>
-      </c>
       <c r="E2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3830,13 +3846,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3844,13 +3860,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3858,13 +3874,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3872,13 +3888,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3886,16 +3902,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D8" t="s">
         <v>407</v>
       </c>
-      <c r="D8" t="s">
-        <v>409</v>
-      </c>
       <c r="E8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3903,13 +3919,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E9" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3917,13 +3933,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3934,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C12" t="s">
+        <v>405</v>
+      </c>
+      <c r="D12" t="s">
         <v>407</v>
       </c>
-      <c r="D12" t="s">
-        <v>409</v>
-      </c>
       <c r="E12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3951,13 +3967,13 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3965,13 +3981,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3979,16 +3995,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D16" t="s">
         <v>407</v>
       </c>
-      <c r="D16" t="s">
-        <v>409</v>
-      </c>
       <c r="E16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3996,13 +4012,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E17" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4010,13 +4026,13 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D18" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E18" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4024,13 +4040,13 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4038,27 +4054,27 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D20" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E23" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -4066,13 +4082,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D24" t="s">
+        <v>500</v>
+      </c>
+      <c r="E24" t="s">
         <v>502</v>
-      </c>
-      <c r="E24" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -4080,13 +4096,13 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E25" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -4094,13 +4110,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D26" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E26" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4108,13 +4124,13 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D27" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E27" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4122,13 +4138,13 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E28" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4136,13 +4152,13 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D29" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E29" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -4150,13 +4166,13 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E30" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4164,13 +4180,13 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D31" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E31" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -4178,13 +4194,13 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D32" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E32" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4192,13 +4208,13 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D33" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E33" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -4206,13 +4222,13 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D34" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E34" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4220,13 +4236,13 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D35" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E35" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -4234,13 +4250,13 @@
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D36" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E36" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -4248,13 +4264,13 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E37" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -4262,13 +4278,13 @@
         <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E38" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -4276,13 +4292,13 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D39" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E39" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -4290,13 +4306,13 @@
         <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D40" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E40" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -4304,13 +4320,13 @@
         <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D41" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E41" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4318,13 +4334,13 @@
         <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D42" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E42" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -4332,13 +4348,13 @@
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D43" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E43" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -4346,13 +4362,13 @@
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D44" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E44" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -4360,13 +4376,13 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D45" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E45" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -4374,13 +4390,13 @@
         <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D46" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E46" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -4388,13 +4404,13 @@
         <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D47" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E47" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -4402,13 +4418,13 @@
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D48" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E48" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4416,13 +4432,13 @@
         <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D49" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E49" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4434,10 +4450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4465,7 +4481,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
@@ -4479,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -4488,13 +4504,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4508,13 +4524,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4528,13 +4544,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4548,13 +4564,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4565,7 +4581,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
         <v>55</v>
@@ -4574,7 +4590,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4588,16 +4604,16 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4605,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -4614,13 +4630,13 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="33">
@@ -4631,16 +4647,16 @@
         <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="33">
@@ -4651,16 +4667,16 @@
         <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="49.5">
@@ -4668,19 +4684,19 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="33">
@@ -4691,16 +4707,16 @@
         <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4714,13 +4730,13 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="33">
@@ -4731,16 +4747,16 @@
         <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4751,16 +4767,16 @@
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="33">
@@ -4771,16 +4787,16 @@
         <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F18" t="s">
+        <v>383</v>
+      </c>
+      <c r="G18" t="s">
         <v>176</v>
-      </c>
-      <c r="E18" t="s">
-        <v>254</v>
-      </c>
-      <c r="F18" t="s">
-        <v>385</v>
-      </c>
-      <c r="G18" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4791,16 +4807,16 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4811,16 +4827,16 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G20" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4831,16 +4847,16 @@
         <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4851,16 +4867,16 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F22" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="33">
@@ -4871,16 +4887,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F23" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="99">
@@ -4891,16 +4907,16 @@
         <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G24" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4911,16 +4927,16 @@
         <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4931,16 +4947,16 @@
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F26" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -4951,16 +4967,16 @@
         <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -4971,16 +4987,16 @@
         <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s">
         <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -4991,16 +5007,16 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F29" t="s">
         <v>18</v>
       </c>
       <c r="G29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5011,16 +5027,16 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="33">
@@ -5031,16 +5047,16 @@
         <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E31" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5051,16 +5067,16 @@
         <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5071,16 +5087,16 @@
         <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F33" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5088,70 +5104,70 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E34" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="C35" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D35" t="s">
+        <v>446</v>
+      </c>
+      <c r="E35" t="s">
+        <v>253</v>
+      </c>
+      <c r="F35" t="s">
+        <v>447</v>
+      </c>
+      <c r="G35" t="s">
         <v>448</v>
-      </c>
-      <c r="E35" t="s">
-        <v>255</v>
-      </c>
-      <c r="F35" t="s">
-        <v>449</v>
-      </c>
-      <c r="G35" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="C36" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D36" t="s">
+        <v>449</v>
+      </c>
+      <c r="E36" t="s">
+        <v>252</v>
+      </c>
+      <c r="F36" t="s">
         <v>451</v>
       </c>
-      <c r="E36" t="s">
-        <v>254</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>453</v>
-      </c>
-      <c r="G36" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="C37" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D37" t="s">
+        <v>450</v>
+      </c>
+      <c r="E37" t="s">
+        <v>252</v>
+      </c>
+      <c r="F37" t="s">
         <v>452</v>
       </c>
-      <c r="E37" t="s">
-        <v>254</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>454</v>
-      </c>
-      <c r="G37" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="49.5">
@@ -5162,962 +5178,1022 @@
         <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E38" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="33">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>569</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E39" t="s">
+        <v>252</v>
+      </c>
+      <c r="F39" t="s">
+        <v>571</v>
+      </c>
+      <c r="G39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="49.5">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>570</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" t="s">
+        <v>252</v>
+      </c>
+      <c r="F40" t="s">
+        <v>571</v>
+      </c>
+      <c r="G40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="33">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" t="s">
+        <v>252</v>
+      </c>
+      <c r="F41" t="s">
+        <v>571</v>
+      </c>
+      <c r="G41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="33">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>413</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="33">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>415</v>
-      </c>
-      <c r="C40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="E43" t="s">
+        <v>252</v>
+      </c>
+      <c r="F43" t="s">
+        <v>393</v>
+      </c>
+      <c r="G43" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="49.5">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E44" t="s">
+        <v>252</v>
+      </c>
+      <c r="F44" t="s">
+        <v>395</v>
+      </c>
+      <c r="G44" t="s">
         <v>191</v>
       </c>
-      <c r="E40" t="s">
-        <v>254</v>
-      </c>
-      <c r="F40" t="s">
-        <v>395</v>
-      </c>
-      <c r="G40" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="49.5">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="E41" t="s">
-        <v>254</v>
-      </c>
-      <c r="F41" t="s">
-        <v>397</v>
-      </c>
-      <c r="G41" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="33">
-      <c r="A42">
+    </row>
+    <row r="45" spans="1:7" ht="33">
+      <c r="A45">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E42" t="s">
-        <v>254</v>
-      </c>
-      <c r="F42" t="s">
-        <v>213</v>
-      </c>
-      <c r="G42" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" t="s">
-        <v>254</v>
-      </c>
-      <c r="F43" t="s">
-        <v>399</v>
-      </c>
-      <c r="G43" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" t="s">
-        <v>117</v>
-      </c>
-      <c r="E44" t="s">
-        <v>254</v>
-      </c>
-      <c r="F44" t="s">
-        <v>400</v>
-      </c>
-      <c r="G44" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <v>6</v>
-      </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" t="s">
-        <v>118</v>
+      <c r="D45" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E45" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F45" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G45" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E46" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F46" t="s">
-        <v>215</v>
+        <v>397</v>
       </c>
       <c r="G46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E47" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F47" t="s">
-        <v>216</v>
+        <v>398</v>
       </c>
       <c r="G47" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E48" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F48" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G48" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>527</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F49" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F50" t="s">
-        <v>471</v>
+        <v>214</v>
       </c>
       <c r="G50" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E51" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F51" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G51" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>525</v>
       </c>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F52" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G52" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E53" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>469</v>
       </c>
       <c r="G53" t="s">
-        <v>205</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>12</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" t="s">
+        <v>122</v>
+      </c>
+      <c r="E54" t="s">
+        <v>252</v>
+      </c>
+      <c r="F54" t="s">
+        <v>217</v>
+      </c>
+      <c r="G54" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
-        <v>401</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F55" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G55" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F56" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="G56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57">
-        <v>3</v>
-      </c>
-      <c r="C57" t="s">
-        <v>129</v>
-      </c>
-      <c r="D57" t="s">
-        <v>131</v>
-      </c>
-      <c r="E57" t="s">
-        <v>254</v>
-      </c>
-      <c r="F57" t="s">
-        <v>222</v>
-      </c>
-      <c r="G57" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>399</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" t="s">
+        <v>252</v>
+      </c>
+      <c r="F58" t="s">
+        <v>209</v>
+      </c>
+      <c r="G58" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" t="s">
+        <v>252</v>
+      </c>
+      <c r="F59" t="s">
+        <v>210</v>
+      </c>
+      <c r="G59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" t="s">
+        <v>252</v>
+      </c>
+      <c r="F60" t="s">
+        <v>220</v>
+      </c>
+      <c r="G60" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
         <v>4</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C61" t="s">
         <v>75</v>
       </c>
-      <c r="D58" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" t="s">
-        <v>254</v>
-      </c>
-      <c r="F58" t="s">
-        <v>472</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="D61" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" t="s">
+        <v>252</v>
+      </c>
+      <c r="F61" t="s">
+        <v>470</v>
+      </c>
+      <c r="G61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="33">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62" t="s">
+        <v>252</v>
+      </c>
+      <c r="F62" t="s">
+        <v>221</v>
+      </c>
+      <c r="G62" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="49.5">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>568</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="33">
-      <c r="A59">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E59" t="s">
-        <v>254</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E63" t="s">
+        <v>252</v>
+      </c>
+      <c r="F63" t="s">
+        <v>222</v>
+      </c>
+      <c r="G63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="33">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>567</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>252</v>
+      </c>
+      <c r="F64" t="s">
         <v>223</v>
       </c>
-      <c r="G59" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="49.5">
-      <c r="A60">
-        <v>6</v>
-      </c>
-      <c r="C60" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" t="s">
-        <v>254</v>
-      </c>
-      <c r="F60" t="s">
-        <v>224</v>
-      </c>
-      <c r="G60" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="33">
-      <c r="A61">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E61" t="s">
-        <v>254</v>
-      </c>
-      <c r="F61" t="s">
-        <v>225</v>
-      </c>
-      <c r="G61" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62">
-        <v>8</v>
-      </c>
-      <c r="C62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62" t="s">
-        <v>133</v>
-      </c>
-      <c r="E62" t="s">
-        <v>254</v>
-      </c>
-      <c r="F62" t="s">
-        <v>226</v>
-      </c>
-      <c r="G62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
-        <v>80</v>
-      </c>
-      <c r="D63" t="s">
-        <v>134</v>
-      </c>
-      <c r="E63" t="s">
-        <v>254</v>
-      </c>
-      <c r="F63" t="s">
-        <v>227</v>
-      </c>
-      <c r="G63" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64">
-        <v>10</v>
-      </c>
-      <c r="C64" t="s">
-        <v>81</v>
-      </c>
-      <c r="D64" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" t="s">
-        <v>254</v>
-      </c>
-      <c r="F64" t="s">
-        <v>228</v>
-      </c>
       <c r="G64" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E65" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F65" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G65" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>230</v>
+        <v>78</v>
       </c>
       <c r="D66" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E66" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F66" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D67" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E67" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F67" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D68" t="s">
-        <v>568</v>
+        <v>134</v>
       </c>
       <c r="E68" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F68" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G68" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="D69" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F69" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G69" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D70" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E70" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F70" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G70" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>566</v>
       </c>
       <c r="E71" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F71" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G71" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E72" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F72" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E73" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F73" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G73" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D74" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E74" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F74" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E75" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F75" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D76" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F76" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G76" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F77" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G77" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D78" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E78" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F78" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G78" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E79" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F79" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G79" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D80" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E80" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F80" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G80" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D81" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E81" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F81" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D82" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E82" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F82" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G82" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C83" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D83" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E83" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F83" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C84" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D84" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E84" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F84" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G84" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C85" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D85" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F85" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="D86" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F86" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G86" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87">
+        <v>30</v>
+      </c>
+      <c r="C87" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" t="s">
+        <v>152</v>
+      </c>
+      <c r="E87" t="s">
+        <v>252</v>
+      </c>
+      <c r="F87" t="s">
+        <v>247</v>
+      </c>
+      <c r="G87" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>31</v>
+      </c>
+      <c r="C88" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" t="s">
+        <v>153</v>
+      </c>
+      <c r="E88" t="s">
+        <v>252</v>
+      </c>
+      <c r="F88" t="s">
+        <v>248</v>
+      </c>
+      <c r="G88" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>32</v>
+      </c>
+      <c r="C89" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" t="s">
+        <v>155</v>
+      </c>
+      <c r="E89" t="s">
+        <v>252</v>
+      </c>
+      <c r="F89" t="s">
+        <v>249</v>
+      </c>
+      <c r="G89" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90">
         <v>33</v>
       </c>
-      <c r="C87" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" t="s">
-        <v>466</v>
-      </c>
-      <c r="E87" t="s">
-        <v>254</v>
-      </c>
-      <c r="F87" t="s">
-        <v>252</v>
-      </c>
-      <c r="G87" t="s">
-        <v>205</v>
+      <c r="C90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" t="s">
+        <v>464</v>
+      </c>
+      <c r="E90" t="s">
+        <v>252</v>
+      </c>
+      <c r="F90" t="s">
+        <v>250</v>
+      </c>
+      <c r="G90" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -6160,7 +6236,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
@@ -6174,7 +6250,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -6183,13 +6259,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6203,13 +6279,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6223,13 +6299,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6243,13 +6319,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6260,7 +6336,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
         <v>55</v>
@@ -6269,7 +6345,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6283,16 +6359,16 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6300,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -6309,13 +6385,13 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6323,19 +6399,19 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="E11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6346,16 +6422,16 @@
         <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6366,16 +6442,16 @@
         <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6386,16 +6462,16 @@
         <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6406,16 +6482,16 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6423,19 +6499,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" t="s">
         <v>270</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E16" t="s">
-        <v>254</v>
-      </c>
-      <c r="F16" t="s">
-        <v>272</v>
-      </c>
       <c r="G16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -6443,19 +6519,19 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" t="s">
         <v>273</v>
       </c>
-      <c r="D17" t="s">
-        <v>275</v>
-      </c>
       <c r="E17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="33">
@@ -6463,19 +6539,19 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="E18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F18" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G18" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -6518,7 +6594,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
@@ -6532,7 +6608,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -6541,13 +6617,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6561,13 +6637,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6581,13 +6657,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6601,13 +6677,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6618,7 +6694,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
         <v>55</v>
@@ -6627,7 +6703,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6641,16 +6717,16 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6658,7 +6734,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -6667,13 +6743,13 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6684,16 +6760,16 @@
         <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6704,16 +6780,16 @@
         <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6724,16 +6800,16 @@
         <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -6744,16 +6820,16 @@
         <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6764,16 +6840,16 @@
         <v>45</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="33">
@@ -6784,16 +6860,16 @@
         <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="82.5">
@@ -6804,16 +6880,16 @@
         <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="33">
@@ -6824,16 +6900,16 @@
         <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="33">
@@ -6841,19 +6917,19 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E19" t="s">
+        <v>285</v>
+      </c>
+      <c r="F19" t="s">
         <v>287</v>
       </c>
-      <c r="F19" t="s">
-        <v>289</v>
-      </c>
       <c r="G19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="49.5">
@@ -6861,19 +6937,19 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F20" t="s">
         <v>290</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E20" t="s">
-        <v>285</v>
-      </c>
-      <c r="F20" t="s">
-        <v>292</v>
-      </c>
       <c r="G20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -6881,19 +6957,19 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F21" t="s">
         <v>293</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E21" t="s">
-        <v>254</v>
-      </c>
-      <c r="F21" t="s">
-        <v>295</v>
-      </c>
       <c r="G21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="33">
@@ -6901,19 +6977,19 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G22" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="33">
@@ -6921,19 +6997,19 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -6941,19 +7017,19 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
+        <v>301</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E24" t="s">
         <v>303</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="F24" t="s">
         <v>304</v>
       </c>
-      <c r="E24" t="s">
-        <v>305</v>
-      </c>
-      <c r="F24" t="s">
-        <v>306</v>
-      </c>
       <c r="G24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="33">
@@ -6961,19 +7037,19 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E25" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" t="s">
         <v>307</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E25" t="s">
-        <v>311</v>
-      </c>
-      <c r="F25" t="s">
-        <v>309</v>
-      </c>
       <c r="G25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="33">
@@ -6981,19 +7057,19 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
+        <v>308</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E26" t="s">
+        <v>252</v>
+      </c>
+      <c r="F26" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E26" t="s">
-        <v>254</v>
-      </c>
-      <c r="F26" t="s">
-        <v>312</v>
-      </c>
       <c r="G26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -7007,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -7036,7 +7112,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
@@ -7050,7 +7126,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -7059,13 +7135,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -7079,13 +7155,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7099,13 +7175,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7119,13 +7195,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7136,7 +7212,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
         <v>55</v>
@@ -7145,7 +7221,7 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7159,16 +7235,16 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7176,7 +7252,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -7185,13 +7261,13 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7202,16 +7278,16 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7222,16 +7298,16 @@
         <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -7242,16 +7318,16 @@
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -7259,19 +7335,19 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" t="s">
         <v>328</v>
       </c>
-      <c r="E14" t="s">
-        <v>254</v>
-      </c>
-      <c r="F14" t="s">
-        <v>330</v>
-      </c>
       <c r="G14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -7279,19 +7355,19 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -7299,19 +7375,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" t="s">
+        <v>309</v>
+      </c>
+      <c r="F16" t="s">
         <v>334</v>
       </c>
-      <c r="D16" t="s">
-        <v>335</v>
-      </c>
-      <c r="E16" t="s">
-        <v>311</v>
-      </c>
-      <c r="F16" t="s">
-        <v>336</v>
-      </c>
       <c r="G16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="33">
@@ -7319,19 +7395,19 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E17" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" t="s">
         <v>337</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E17" t="s">
-        <v>287</v>
-      </c>
-      <c r="F17" t="s">
-        <v>339</v>
-      </c>
       <c r="G17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="33">
@@ -7339,19 +7415,19 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F18" t="s">
         <v>341</v>
       </c>
-      <c r="E18" t="s">
-        <v>254</v>
-      </c>
-      <c r="F18" t="s">
-        <v>343</v>
-      </c>
       <c r="G18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -7359,19 +7435,19 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G19" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -7379,19 +7455,19 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F20" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G20" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="33">
@@ -7399,22 +7475,22 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C22" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F22" t="s">
         <v>349</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E22" t="s">
-        <v>254</v>
-      </c>
-      <c r="F22" t="s">
-        <v>351</v>
-      </c>
       <c r="G22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="33">
@@ -7422,19 +7498,19 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="49.5">
@@ -7442,19 +7518,19 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>352</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>356</v>
-      </c>
       <c r="E24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="49.5">
@@ -7462,19 +7538,19 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -7482,19 +7558,19 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
+        <v>359</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E26" t="s">
+        <v>377</v>
+      </c>
+      <c r="F26" t="s">
         <v>361</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E26" t="s">
-        <v>379</v>
-      </c>
-      <c r="F26" t="s">
-        <v>363</v>
-      </c>
       <c r="G26" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -7502,22 +7578,22 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G28" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="33">
@@ -7525,19 +7601,19 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F29" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -7545,19 +7621,19 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -7565,19 +7641,19 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
+        <v>376</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="E31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>